<commit_message>
just updating the sulfate data for reservoirs and assay experiment combined now
</commit_message>
<xml_diff>
--- a/Assay Experiment/assay_sulfate_data.xlsx
+++ b/Assay Experiment/assay_sulfate_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c9f30cf11edfc58c/2023 Rtudio/Reservoirs_sulfate/Assay Experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="590" documentId="8_{F11D555E-D919-4B61-AB1E-2561B0A8B23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABB47961-F31C-4CCD-A030-0A7C6B59DB00}"/>
+  <xr:revisionPtr revIDLastSave="793" documentId="8_{F11D555E-D919-4B61-AB1E-2561B0A8B23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6842A16E-E563-4F69-9379-993CAE7C8AEC}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="372" windowWidth="15108" windowHeight="10752" tabRatio="845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="19" r:id="rId1"/>
@@ -888,7 +888,7 @@
       <name val="MS Sans Serif"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -915,6 +915,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1115,7 +1121,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1453,6 +1459,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5448,11 +5457,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF79B75-9ED3-461B-AB3B-6B685EC2DFDE}">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="121" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="126" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E114" sqref="E114"/>
+      <selection pane="topRight" activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6202,32 +6211,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>178</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38" s="146">
-        <v>45859</v>
-      </c>
-      <c r="E38" s="33">
-        <v>1167.1474955333704</v>
-      </c>
-      <c r="F38">
-        <v>2</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
-        <v>214</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -6238,22 +6224,22 @@
       <c r="D39" s="146">
         <v>45859</v>
       </c>
-      <c r="E39" s="33">
-        <v>1436.3245729448201</v>
+      <c r="E39">
+        <v>1063</v>
       </c>
       <c r="F39">
         <v>2</v>
       </c>
       <c r="G39">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
-        <v>175</v>
+      <c r="A40" t="s">
+        <v>214</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -6261,19 +6247,19 @@
       <c r="D40" s="146">
         <v>45859</v>
       </c>
-      <c r="E40" s="33">
-        <v>2453.6629021675058</v>
+      <c r="E40">
+        <v>1312</v>
       </c>
       <c r="F40">
         <v>2</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
-        <v>233</v>
+      <c r="A41" t="s">
+        <v>175</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -6284,22 +6270,22 @@
       <c r="D41" s="146">
         <v>45859</v>
       </c>
-      <c r="E41" s="33">
-        <v>1022.9195062350911</v>
+      <c r="E41">
+        <v>1020</v>
       </c>
       <c r="F41">
         <v>2</v>
       </c>
       <c r="G41">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
-        <v>180</v>
+      <c r="A42" t="s">
+        <v>233</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -6307,19 +6293,19 @@
       <c r="D42" s="146">
         <v>45859</v>
       </c>
-      <c r="E42" s="33">
-        <v>1180.8496055540013</v>
+      <c r="E42">
+        <v>929</v>
       </c>
       <c r="F42">
         <v>2</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="28" t="s">
-        <v>230</v>
+      <c r="A43" t="s">
+        <v>180</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -6330,22 +6316,22 @@
       <c r="D43" s="146">
         <v>45859</v>
       </c>
-      <c r="E43" s="33">
-        <v>987.50572147254832</v>
+      <c r="E43">
+        <v>1075</v>
       </c>
       <c r="F43">
         <v>2</v>
       </c>
       <c r="G43">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
-        <v>177</v>
+      <c r="A44" t="s">
+        <v>230</v>
       </c>
       <c r="B44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -6353,19 +6339,19 @@
       <c r="D44" s="146">
         <v>45859</v>
       </c>
-      <c r="E44" s="33">
-        <v>1968.0100239954529</v>
+      <c r="E44">
+        <v>896</v>
       </c>
       <c r="F44">
         <v>2</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="s">
-        <v>201</v>
+      <c r="A45" t="s">
+        <v>177</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -6376,22 +6362,22 @@
       <c r="D45" s="146">
         <v>45859</v>
       </c>
-      <c r="E45" s="33">
-        <v>957.11206364546752</v>
+      <c r="E45">
+        <v>1804</v>
       </c>
       <c r="F45">
         <v>2</v>
       </c>
       <c r="G45">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="28" t="s">
-        <v>172</v>
+      <c r="A46" t="s">
+        <v>201</v>
       </c>
       <c r="B46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -6399,19 +6385,19 @@
       <c r="D46" s="146">
         <v>45859</v>
       </c>
-      <c r="E46" s="33">
-        <v>1312.3869059232886</v>
+      <c r="E46">
+        <v>868</v>
       </c>
       <c r="F46">
         <v>2</v>
       </c>
       <c r="G46">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="28" t="s">
-        <v>200</v>
+      <c r="A47" t="s">
+        <v>172</v>
       </c>
       <c r="B47">
         <v>5</v>
@@ -6422,22 +6408,22 @@
       <c r="D47" s="146">
         <v>45859</v>
       </c>
-      <c r="E47" s="33">
-        <v>954.52843675516363</v>
+      <c r="E47">
+        <v>1197</v>
       </c>
       <c r="F47">
         <v>2</v>
       </c>
       <c r="G47">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
-        <v>226</v>
+      <c r="A48" t="s">
+        <v>200</v>
       </c>
       <c r="B48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -6445,19 +6431,19 @@
       <c r="D48" s="146">
         <v>45859</v>
       </c>
-      <c r="E48" s="33">
-        <v>1445.8895424531111</v>
+      <c r="E48">
+        <v>866</v>
       </c>
       <c r="F48">
         <v>2</v>
       </c>
       <c r="G48">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
-        <v>218</v>
+      <c r="A49" t="s">
+        <v>226</v>
       </c>
       <c r="B49">
         <v>6</v>
@@ -6468,42 +6454,42 @@
       <c r="D49" s="146">
         <v>45859</v>
       </c>
-      <c r="E49" s="33">
-        <v>1261.00612327196</v>
+      <c r="E49">
+        <v>1321</v>
       </c>
       <c r="F49">
         <v>2</v>
       </c>
       <c r="G49">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
-        <v>228</v>
+      <c r="A50" t="s">
+        <v>218</v>
       </c>
       <c r="B50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C50">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D50" s="146">
         <v>45859</v>
       </c>
-      <c r="E50" s="33">
-        <v>1751.2570503261518</v>
+      <c r="E50">
+        <v>1150</v>
       </c>
       <c r="F50">
         <v>2</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
-        <v>186</v>
+      <c r="A51" t="s">
+        <v>228</v>
       </c>
       <c r="B51">
         <v>7</v>
@@ -6514,22 +6500,22 @@
       <c r="D51" s="146">
         <v>45859</v>
       </c>
-      <c r="E51" s="33">
-        <v>1558.6061921867772</v>
+      <c r="E51">
+        <v>1604</v>
       </c>
       <c r="F51">
         <v>2</v>
       </c>
       <c r="G51">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
-        <v>225</v>
+      <c r="A52" t="s">
+        <v>186</v>
       </c>
       <c r="B52">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C52">
         <v>0.5</v>
@@ -6537,19 +6523,19 @@
       <c r="D52" s="146">
         <v>45859</v>
       </c>
-      <c r="E52" s="33">
-        <v>1679.4230140904544</v>
+      <c r="E52">
+        <v>1425</v>
       </c>
       <c r="F52">
         <v>2</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="28" t="s">
-        <v>217</v>
+      <c r="A53" t="s">
+        <v>225</v>
       </c>
       <c r="B53">
         <v>8</v>
@@ -6560,22 +6546,22 @@
       <c r="D53" s="146">
         <v>45859</v>
       </c>
-      <c r="E53" s="33">
-        <v>1547.0857998410338</v>
+      <c r="E53">
+        <v>1537</v>
       </c>
       <c r="F53">
         <v>2</v>
       </c>
       <c r="G53">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
-        <v>173</v>
+      <c r="A54" t="s">
+        <v>217</v>
       </c>
       <c r="B54">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C54">
         <v>0.5</v>
@@ -6583,19 +6569,19 @@
       <c r="D54" s="146">
         <v>45859</v>
       </c>
-      <c r="E54" s="33">
-        <v>2025.5443741843333</v>
+      <c r="E54">
+        <v>1415</v>
       </c>
       <c r="F54">
         <v>2</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
-        <v>167</v>
+      <c r="A55" t="s">
+        <v>173</v>
       </c>
       <c r="B55">
         <v>9</v>
@@ -6606,22 +6592,22 @@
       <c r="D55" s="146">
         <v>45859</v>
       </c>
-      <c r="E55" s="33">
-        <v>1544.0184121381535</v>
+      <c r="E55">
+        <v>1858</v>
       </c>
       <c r="F55">
         <v>2</v>
       </c>
       <c r="G55">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="s">
-        <v>198</v>
+      <c r="A56" t="s">
+        <v>167</v>
       </c>
       <c r="B56">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C56">
         <v>0.5</v>
@@ -6629,19 +6615,19 @@
       <c r="D56" s="146">
         <v>45859</v>
       </c>
-      <c r="E56" s="33">
-        <v>1705.1817625823837</v>
+      <c r="E56">
+        <v>1412</v>
       </c>
       <c r="F56">
         <v>2</v>
       </c>
       <c r="G56">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="28" t="s">
-        <v>212</v>
+      <c r="A57" t="s">
+        <v>198</v>
       </c>
       <c r="B57">
         <v>10</v>
@@ -6652,22 +6638,22 @@
       <c r="D57" s="146">
         <v>45859</v>
       </c>
-      <c r="E57" s="33">
-        <v>1548.3785262105666</v>
+      <c r="E57">
+        <v>1561</v>
       </c>
       <c r="F57">
         <v>2</v>
       </c>
       <c r="G57">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="s">
-        <v>188</v>
+      <c r="A58" t="s">
+        <v>212</v>
       </c>
       <c r="B58">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C58">
         <v>0.5</v>
@@ -6675,19 +6661,19 @@
       <c r="D58" s="146">
         <v>45859</v>
       </c>
-      <c r="E58" s="33">
-        <v>1604.1654994999647</v>
+      <c r="E58">
+        <v>1416</v>
       </c>
       <c r="F58">
         <v>2</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="28" t="s">
-        <v>231</v>
+      <c r="A59" t="s">
+        <v>188</v>
       </c>
       <c r="B59">
         <v>11</v>
@@ -6698,22 +6684,22 @@
       <c r="D59" s="146">
         <v>45859</v>
       </c>
-      <c r="E59" s="33">
-        <v>1537.8073588855932</v>
+      <c r="E59">
+        <v>1467</v>
       </c>
       <c r="F59">
         <v>2</v>
       </c>
       <c r="G59">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="28" t="s">
-        <v>206</v>
+      <c r="A60" t="s">
+        <v>231</v>
       </c>
       <c r="B60">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C60">
         <v>0.5</v>
@@ -6721,19 +6707,19 @@
       <c r="D60" s="146">
         <v>45859</v>
       </c>
-      <c r="E60" s="33">
-        <v>1644.7581170229284</v>
+      <c r="E60">
+        <v>1406</v>
       </c>
       <c r="F60">
         <v>2</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="28" t="s">
-        <v>211</v>
+      <c r="A61" t="s">
+        <v>206</v>
       </c>
       <c r="B61">
         <v>12</v>
@@ -6744,42 +6730,42 @@
       <c r="D61" s="146">
         <v>45859</v>
       </c>
-      <c r="E61" s="33">
-        <v>1628.6620051681643</v>
+      <c r="E61">
+        <v>1505</v>
       </c>
       <c r="F61">
         <v>2</v>
       </c>
       <c r="G61">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="28" t="s">
-        <v>170</v>
+      <c r="A62" t="s">
+        <v>211</v>
       </c>
       <c r="B62">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D62" s="146">
         <v>45859</v>
       </c>
-      <c r="E62" s="33">
-        <v>2342.0028416868508</v>
+      <c r="E62">
+        <v>1490</v>
       </c>
       <c r="F62">
         <v>2</v>
       </c>
       <c r="G62">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="28" t="s">
-        <v>219</v>
+      <c r="A63" t="s">
+        <v>170</v>
       </c>
       <c r="B63">
         <v>13</v>
@@ -6790,22 +6776,22 @@
       <c r="D63" s="146">
         <v>45859</v>
       </c>
-      <c r="E63" s="33">
-        <v>2064.4292926166108</v>
+      <c r="E63">
+        <v>2151</v>
       </c>
       <c r="F63">
         <v>2</v>
       </c>
       <c r="G63">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="28" t="s">
-        <v>227</v>
+      <c r="A64" t="s">
+        <v>219</v>
       </c>
       <c r="B64">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -6813,19 +6799,19 @@
       <c r="D64" s="146">
         <v>45859</v>
       </c>
-      <c r="E64" s="33">
-        <v>2315.7068381986824</v>
+      <c r="E64">
+        <v>1894</v>
       </c>
       <c r="F64">
         <v>2</v>
       </c>
       <c r="G64">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="28" t="s">
-        <v>208</v>
+      <c r="A65" t="s">
+        <v>227</v>
       </c>
       <c r="B65">
         <v>14</v>
@@ -6836,22 +6822,22 @@
       <c r="D65" s="146">
         <v>45859</v>
       </c>
-      <c r="E65" s="33">
-        <v>2052.8834755869239</v>
+      <c r="E65">
+        <v>2126</v>
       </c>
       <c r="F65">
         <v>2</v>
       </c>
       <c r="G65">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="28" t="s">
-        <v>222</v>
+      <c r="A66" t="s">
+        <v>208</v>
       </c>
       <c r="B66">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -6859,19 +6845,19 @@
       <c r="D66" s="146">
         <v>45859</v>
       </c>
-      <c r="E66" s="33">
-        <v>2221.7916051688967</v>
+      <c r="E66">
+        <v>1883</v>
       </c>
       <c r="F66">
         <v>2</v>
       </c>
       <c r="G66">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="28" t="s">
-        <v>209</v>
+      <c r="A67" t="s">
+        <v>222</v>
       </c>
       <c r="B67">
         <v>15</v>
@@ -6882,22 +6868,22 @@
       <c r="D67" s="146">
         <v>45859</v>
       </c>
-      <c r="E67" s="33">
-        <v>2017.3745341311276</v>
+      <c r="E67">
+        <v>2039</v>
       </c>
       <c r="F67">
         <v>2</v>
       </c>
       <c r="G67">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="28" t="s">
-        <v>197</v>
+      <c r="A68" t="s">
+        <v>209</v>
       </c>
       <c r="B68">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -6905,19 +6891,19 @@
       <c r="D68" s="146">
         <v>45859</v>
       </c>
-      <c r="E68" s="33">
-        <v>2202.5764146340657</v>
+      <c r="E68">
+        <v>1850</v>
       </c>
       <c r="F68">
         <v>2</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="28" t="s">
-        <v>203</v>
+      <c r="A69" t="s">
+        <v>197</v>
       </c>
       <c r="B69">
         <v>16</v>
@@ -6928,22 +6914,22 @@
       <c r="D69" s="146">
         <v>45859</v>
       </c>
-      <c r="E69" s="33">
-        <v>2077.542296923677</v>
+      <c r="E69">
+        <v>2022</v>
       </c>
       <c r="F69">
         <v>2</v>
       </c>
       <c r="G69">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="28" t="s">
-        <v>192</v>
+      <c r="A70" t="s">
+        <v>203</v>
       </c>
       <c r="B70">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -6951,19 +6937,19 @@
       <c r="D70" s="146">
         <v>45859</v>
       </c>
-      <c r="E70" s="33">
-        <v>2055.5772759003657</v>
+      <c r="E70">
+        <v>1906</v>
       </c>
       <c r="F70">
         <v>2</v>
       </c>
       <c r="G70">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="28" t="s">
-        <v>229</v>
+      <c r="A71" t="s">
+        <v>192</v>
       </c>
       <c r="B71">
         <v>17</v>
@@ -6974,22 +6960,22 @@
       <c r="D71" s="146">
         <v>45859</v>
       </c>
-      <c r="E71" s="33">
-        <v>2179.8716785816168</v>
+      <c r="E71">
+        <v>1885</v>
       </c>
       <c r="F71">
         <v>2</v>
       </c>
       <c r="G71">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="28" t="s">
-        <v>184</v>
+      <c r="A72" t="s">
+        <v>229</v>
       </c>
       <c r="B72">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -6997,65 +6983,65 @@
       <c r="D72" s="146">
         <v>45859</v>
       </c>
-      <c r="E72" s="33">
-        <v>1873.8127566302135</v>
+      <c r="E72">
+        <v>2001</v>
       </c>
       <c r="F72">
         <v>2</v>
       </c>
       <c r="G72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="147" t="s">
+        <v>224</v>
+      </c>
+      <c r="B73" s="147">
+        <v>18</v>
+      </c>
+      <c r="C73" s="147">
         <v>1</v>
       </c>
+      <c r="D73" s="148">
+        <v>45859</v>
+      </c>
+      <c r="E73" s="147">
+        <v>1717</v>
+      </c>
+      <c r="F73" s="147">
+        <v>2</v>
+      </c>
+      <c r="G73" s="147">
+        <v>2</v>
+      </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="28" t="s">
-        <v>224</v>
-      </c>
-      <c r="B73">
+    <row r="74" spans="1:7" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="147" t="s">
+        <v>184</v>
+      </c>
+      <c r="B74" s="147">
         <v>18</v>
       </c>
-      <c r="C73">
+      <c r="C74" s="147">
         <v>1</v>
       </c>
-      <c r="D73" s="146">
+      <c r="D74" s="148">
         <v>45859</v>
       </c>
-      <c r="E73" s="33">
-        <v>2120.2176179725816</v>
-      </c>
-      <c r="F73">
+      <c r="E74" s="147">
+        <v>1945</v>
+      </c>
+      <c r="F74" s="147">
         <v>2</v>
       </c>
-      <c r="G73">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="B74">
-        <v>19</v>
-      </c>
-      <c r="C74">
-        <v>3</v>
-      </c>
-      <c r="D74" s="146">
-        <v>45859</v>
-      </c>
-      <c r="E74" s="33">
-        <v>4999.8614765285492</v>
-      </c>
-      <c r="F74">
-        <v>2</v>
-      </c>
-      <c r="G74">
+      <c r="G74" s="147">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="28" t="s">
-        <v>221</v>
+      <c r="A75" t="s">
+        <v>176</v>
       </c>
       <c r="B75">
         <v>19</v>
@@ -7066,22 +7052,22 @@
       <c r="D75" s="146">
         <v>45859</v>
       </c>
-      <c r="E75" s="33">
-        <v>4601.803859944891</v>
+      <c r="E75">
+        <v>4612</v>
       </c>
       <c r="F75">
         <v>2</v>
       </c>
       <c r="G75">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="28" t="s">
-        <v>165</v>
+      <c r="A76" t="s">
+        <v>221</v>
       </c>
       <c r="B76">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C76">
         <v>3</v>
@@ -7089,65 +7075,65 @@
       <c r="D76" s="146">
         <v>45859</v>
       </c>
-      <c r="E76" s="33">
-        <v>4477.2240828036147</v>
+      <c r="E76">
+        <v>4243</v>
       </c>
       <c r="F76">
         <v>2</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="28" t="s">
-        <v>210</v>
+      <c r="A77" t="s">
+        <v>165</v>
       </c>
       <c r="B77">
         <v>20</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="147">
         <v>3</v>
       </c>
       <c r="D77" s="146">
         <v>45859</v>
       </c>
-      <c r="E77" s="33">
-        <v>4294.7472965808793</v>
+      <c r="E77">
+        <v>4128</v>
       </c>
       <c r="F77">
         <v>2</v>
       </c>
       <c r="G77">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="28" t="s">
-        <v>193</v>
+      <c r="A78" t="s">
+        <v>210</v>
       </c>
       <c r="B78">
-        <v>21</v>
-      </c>
-      <c r="C78">
+        <v>20</v>
+      </c>
+      <c r="C78" s="147">
         <v>3</v>
       </c>
       <c r="D78" s="146">
         <v>45859</v>
       </c>
-      <c r="E78" s="33">
-        <v>3722.2815372349314</v>
+      <c r="E78">
+        <v>3959</v>
       </c>
       <c r="F78">
         <v>2</v>
       </c>
       <c r="G78">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="28" t="s">
-        <v>195</v>
+      <c r="A79" t="s">
+        <v>193</v>
       </c>
       <c r="B79">
         <v>21</v>
@@ -7158,22 +7144,22 @@
       <c r="D79" s="146">
         <v>45859</v>
       </c>
-      <c r="E79" s="33">
-        <v>4222.1112861872962</v>
+      <c r="E79">
+        <v>3429</v>
       </c>
       <c r="F79">
         <v>2</v>
       </c>
       <c r="G79">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="28" t="s">
-        <v>235</v>
+      <c r="A80" t="s">
+        <v>195</v>
       </c>
       <c r="B80">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C80">
         <v>3</v>
@@ -7181,31 +7167,31 @@
       <c r="D80" s="146">
         <v>45859</v>
       </c>
-      <c r="E80" s="33">
-        <v>4507.7899365950061</v>
+      <c r="E80">
+        <v>3892</v>
       </c>
       <c r="F80">
         <v>2</v>
       </c>
       <c r="G80">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="28" t="s">
+      <c r="A81" t="s">
         <v>204</v>
       </c>
       <c r="B81">
         <v>22</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="147">
         <v>3</v>
       </c>
       <c r="D81" s="146">
         <v>45859</v>
       </c>
-      <c r="E81" s="33">
-        <v>4429.3664122517312</v>
+      <c r="E81">
+        <v>4084</v>
       </c>
       <c r="F81">
         <v>2</v>
@@ -7214,58 +7200,58 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="28" t="s">
+    <row r="82" spans="1:7" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="84" t="s">
         <v>185</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="84">
         <v>23</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="147">
         <v>3</v>
       </c>
-      <c r="D82" s="146">
+      <c r="D82" s="149">
         <v>45859</v>
       </c>
-      <c r="E82" s="33">
-        <v>3410.1338211546845</v>
-      </c>
-      <c r="F82">
+      <c r="E82" s="84">
+        <v>3140</v>
+      </c>
+      <c r="F82" s="84">
         <v>2</v>
       </c>
-      <c r="G82">
+      <c r="G82" s="84">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="B83">
-        <v>23</v>
+    <row r="83" spans="1:7" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="84" t="s">
+        <v>235</v>
+      </c>
+      <c r="B83" s="84">
+        <v>22</v>
       </c>
       <c r="C83">
         <v>3</v>
       </c>
-      <c r="D83" s="146">
+      <c r="D83" s="149">
         <v>45859</v>
       </c>
-      <c r="E83" s="33">
-        <v>4525.7239397794701</v>
-      </c>
-      <c r="F83">
+      <c r="E83" s="84">
+        <v>4156</v>
+      </c>
+      <c r="F83" s="84">
         <v>2</v>
       </c>
-      <c r="G83">
-        <v>2</v>
+      <c r="G83" s="84">
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="28" t="s">
-        <v>216</v>
+      <c r="A84" t="s">
+        <v>232</v>
       </c>
       <c r="B84">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C84">
         <v>3</v>
@@ -7273,353 +7259,353 @@
       <c r="D84" s="146">
         <v>45859</v>
       </c>
-      <c r="E84" s="33">
-        <v>4104.4545412488678</v>
+      <c r="E84">
+        <v>4173</v>
       </c>
       <c r="F84">
         <v>2</v>
       </c>
       <c r="G84">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="28" t="s">
-        <v>215</v>
+      <c r="A85" t="s">
+        <v>216</v>
       </c>
       <c r="B85">
         <v>24</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="147">
         <v>3</v>
       </c>
       <c r="D85" s="146">
         <v>45859</v>
       </c>
-      <c r="E85" s="33">
-        <v>4425.5760761859092</v>
+      <c r="E85">
+        <v>3783</v>
       </c>
       <c r="F85">
         <v>2</v>
       </c>
       <c r="G85">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="28" t="s">
-        <v>199</v>
+      <c r="A86" t="s">
+        <v>215</v>
       </c>
       <c r="B86">
-        <v>25</v>
-      </c>
-      <c r="C86">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="C86" s="147">
+        <v>3</v>
       </c>
       <c r="D86" s="146">
         <v>45859</v>
       </c>
-      <c r="E86" s="33">
-        <v>5763.679055363963</v>
+      <c r="E86">
+        <v>4080</v>
       </c>
       <c r="F86">
         <v>2</v>
       </c>
       <c r="G86">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="28" t="s">
-        <v>220</v>
+      <c r="A87" t="s">
+        <v>199</v>
       </c>
       <c r="B87">
         <v>25</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="147">
         <v>5</v>
       </c>
       <c r="D87" s="146">
         <v>45859</v>
       </c>
-      <c r="E87" s="33">
-        <v>6529.860633530182</v>
+      <c r="E87">
+        <v>5319</v>
       </c>
       <c r="F87">
         <v>2</v>
       </c>
       <c r="G87">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="28" t="s">
-        <v>196</v>
+      <c r="A88" t="s">
+        <v>220</v>
       </c>
       <c r="B88">
-        <v>26</v>
-      </c>
-      <c r="C88">
+        <v>25</v>
+      </c>
+      <c r="C88" s="147">
         <v>5</v>
       </c>
       <c r="D88" s="146">
         <v>45859</v>
       </c>
-      <c r="E88" s="33">
-        <v>5791.0994560071103</v>
+      <c r="E88">
+        <v>6028</v>
       </c>
       <c r="F88">
         <v>2</v>
       </c>
       <c r="G88">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="28" t="s">
-        <v>168</v>
+      <c r="A89" t="s">
+        <v>196</v>
       </c>
       <c r="B89">
         <v>26</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="147">
         <v>5</v>
       </c>
       <c r="D89" s="146">
         <v>45859</v>
       </c>
-      <c r="E89" s="33">
-        <v>6571.7564685938705</v>
+      <c r="E89">
+        <v>5344</v>
       </c>
       <c r="F89">
         <v>2</v>
       </c>
       <c r="G89">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="28" t="s">
-        <v>187</v>
+      <c r="A90" t="s">
+        <v>168</v>
       </c>
       <c r="B90">
-        <v>27</v>
-      </c>
-      <c r="C90">
+        <v>26</v>
+      </c>
+      <c r="C90" s="147">
         <v>5</v>
       </c>
       <c r="D90" s="146">
         <v>45859</v>
       </c>
-      <c r="E90" s="33">
-        <v>6041.9714472139831</v>
+      <c r="E90">
+        <v>6067</v>
       </c>
       <c r="F90">
         <v>2</v>
       </c>
       <c r="G90">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="28" t="s">
-        <v>234</v>
+      <c r="A91" t="s">
+        <v>187</v>
       </c>
       <c r="B91">
         <v>27</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="147">
         <v>5</v>
       </c>
       <c r="D91" s="146">
         <v>45859</v>
       </c>
-      <c r="E91" s="33">
-        <v>6905.0557988407645</v>
+      <c r="E91">
+        <v>5577</v>
       </c>
       <c r="F91">
         <v>2</v>
       </c>
       <c r="G91">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="28" t="s">
-        <v>207</v>
+      <c r="A92" t="s">
+        <v>234</v>
       </c>
       <c r="B92">
-        <v>28</v>
-      </c>
-      <c r="C92">
+        <v>27</v>
+      </c>
+      <c r="C92" s="147">
         <v>5</v>
       </c>
       <c r="D92" s="146">
         <v>45859</v>
       </c>
-      <c r="E92" s="33">
-        <v>6845.4374701853976</v>
+      <c r="E92">
+        <v>6376</v>
       </c>
       <c r="F92">
         <v>2</v>
       </c>
       <c r="G92">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="28" t="s">
-        <v>202</v>
+      <c r="A93" t="s">
+        <v>207</v>
       </c>
       <c r="B93">
         <v>28</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="147">
         <v>5</v>
       </c>
       <c r="D93" s="146">
         <v>45859</v>
       </c>
-      <c r="E93" s="33">
-        <v>6698.9445974669607</v>
+      <c r="E93">
+        <v>6321</v>
       </c>
       <c r="F93">
         <v>2</v>
       </c>
       <c r="G93">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="28" t="s">
-        <v>194</v>
+      <c r="A94" t="s">
+        <v>202</v>
       </c>
       <c r="B94">
-        <v>29</v>
-      </c>
-      <c r="C94">
+        <v>28</v>
+      </c>
+      <c r="C94" s="147">
         <v>5</v>
       </c>
       <c r="D94" s="146">
         <v>45859</v>
       </c>
-      <c r="E94" s="33">
-        <v>6745.8059754307887</v>
+      <c r="E94">
+        <v>6185</v>
       </c>
       <c r="F94">
         <v>2</v>
       </c>
       <c r="G94">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="28" t="s">
-        <v>223</v>
+      <c r="A95" t="s">
+        <v>194</v>
       </c>
       <c r="B95">
         <v>29</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="147">
         <v>5</v>
       </c>
       <c r="D95" s="146">
         <v>45859</v>
       </c>
-      <c r="E95" s="33">
-        <v>7063.236755712589</v>
+      <c r="E95">
+        <v>6228</v>
       </c>
       <c r="F95">
         <v>2</v>
       </c>
       <c r="G95">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="28" t="s">
-        <v>190</v>
+      <c r="A96" t="s">
+        <v>223</v>
       </c>
       <c r="B96">
-        <v>30</v>
-      </c>
-      <c r="C96">
+        <v>29</v>
+      </c>
+      <c r="C96" s="147">
         <v>5</v>
       </c>
       <c r="D96" s="146">
         <v>45859</v>
       </c>
-      <c r="E96" s="33">
-        <v>6641.4697444101566</v>
+      <c r="E96">
+        <v>6522</v>
       </c>
       <c r="F96">
         <v>2</v>
       </c>
       <c r="G96">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="28" t="s">
-        <v>169</v>
+      <c r="A97" t="s">
+        <v>190</v>
       </c>
       <c r="B97">
         <v>30</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="147">
         <v>5</v>
       </c>
       <c r="D97" s="146">
         <v>45859</v>
       </c>
-      <c r="E97" s="33">
-        <v>6630.3062444907737</v>
+      <c r="E97">
+        <v>6132</v>
       </c>
       <c r="F97">
         <v>2</v>
       </c>
       <c r="G97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="B98" s="84">
+        <v>30</v>
+      </c>
+      <c r="C98" s="147">
+        <v>5</v>
+      </c>
+      <c r="D98" s="149">
+        <v>45859</v>
+      </c>
+      <c r="E98" s="84">
+        <v>6121</v>
+      </c>
+      <c r="F98" s="84">
         <v>2</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="B98">
-        <v>30</v>
-      </c>
-      <c r="C98">
-        <v>7</v>
-      </c>
-      <c r="D98" s="146">
-        <v>45859</v>
-      </c>
-      <c r="E98" s="33">
-        <v>8650.8564575417859</v>
-      </c>
-      <c r="F98">
-        <v>2</v>
-      </c>
-      <c r="G98">
+      <c r="G98" s="84">
         <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="28" t="s">
+      <c r="A99" t="s">
         <v>174</v>
       </c>
       <c r="B99">
         <v>31</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="147">
         <v>7</v>
       </c>
       <c r="D99" s="146">
         <v>45859</v>
       </c>
-      <c r="E99" s="33">
-        <v>9385.8322016372913</v>
+      <c r="E99">
+        <v>8672</v>
       </c>
       <c r="F99">
         <v>2</v>
@@ -7629,20 +7615,20 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="28" t="s">
+      <c r="A100" t="s">
         <v>213</v>
       </c>
       <c r="B100">
         <v>31</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="147">
         <v>7</v>
       </c>
       <c r="D100" s="146">
         <v>45859</v>
       </c>
-      <c r="E100" s="33">
-        <v>9263.4758713053998</v>
+      <c r="E100">
+        <v>8559</v>
       </c>
       <c r="F100">
         <v>2</v>
@@ -7652,20 +7638,20 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="28" t="s">
+      <c r="A101" t="s">
         <v>171</v>
       </c>
       <c r="B101">
         <v>32</v>
       </c>
-      <c r="C101">
+      <c r="C101" s="147">
         <v>7</v>
       </c>
       <c r="D101" s="146">
         <v>45859</v>
       </c>
-      <c r="E101" s="33">
-        <v>11150.572192822647</v>
+      <c r="E101">
+        <v>10306</v>
       </c>
       <c r="F101">
         <v>2</v>
@@ -7675,20 +7661,20 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="28" t="s">
+      <c r="A102" t="s">
         <v>166</v>
       </c>
       <c r="B102">
         <v>32</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="147">
         <v>7</v>
       </c>
       <c r="D102" s="146">
         <v>45859</v>
       </c>
-      <c r="E102" s="33">
-        <v>9010.8606072287876</v>
+      <c r="E102">
+        <v>8325</v>
       </c>
       <c r="F102">
         <v>2</v>
@@ -7698,20 +7684,20 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="28" t="s">
+      <c r="A103" t="s">
         <v>181</v>
       </c>
       <c r="B103">
         <v>33</v>
       </c>
-      <c r="C103">
+      <c r="C103" s="147">
         <v>7</v>
       </c>
       <c r="D103" s="146">
         <v>45859</v>
       </c>
-      <c r="E103" s="33">
-        <v>9649.8493993953798</v>
+      <c r="E103">
+        <v>8917</v>
       </c>
       <c r="F103">
         <v>2</v>
@@ -7721,20 +7707,20 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="28" t="s">
+      <c r="A104" t="s">
         <v>183</v>
       </c>
       <c r="B104">
         <v>33</v>
       </c>
-      <c r="C104">
+      <c r="C104" s="147">
         <v>7</v>
       </c>
       <c r="D104" s="146">
         <v>45859</v>
       </c>
-      <c r="E104" s="33">
-        <v>8642.6169113372234</v>
+      <c r="E104">
+        <v>7984</v>
       </c>
       <c r="F104">
         <v>2</v>
@@ -7744,20 +7730,20 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="28" t="s">
+      <c r="A105" t="s">
         <v>182</v>
       </c>
       <c r="B105">
         <v>34</v>
       </c>
-      <c r="C105">
+      <c r="C105" s="147">
         <v>7</v>
       </c>
       <c r="D105" s="146">
         <v>45859</v>
       </c>
-      <c r="E105" s="33">
-        <v>9125.2585619014608</v>
+      <c r="E105">
+        <v>8431</v>
       </c>
       <c r="F105">
         <v>2</v>
@@ -7767,20 +7753,20 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="28" t="s">
+      <c r="A106" t="s">
         <v>205</v>
       </c>
       <c r="B106">
         <v>34</v>
       </c>
-      <c r="C106">
+      <c r="C106" s="147">
         <v>7</v>
       </c>
       <c r="D106" s="146">
         <v>45859</v>
       </c>
-      <c r="E106" s="33">
-        <v>9072.0024157352618</v>
+      <c r="E106">
+        <v>8382</v>
       </c>
       <c r="F106">
         <v>2</v>
@@ -7790,20 +7776,20 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="28" t="s">
+      <c r="A107" t="s">
         <v>179</v>
       </c>
       <c r="B107">
         <v>35</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="147">
         <v>7</v>
       </c>
       <c r="D107" s="146">
         <v>45859</v>
       </c>
-      <c r="E107" s="33">
-        <v>8826.1624035629575</v>
+      <c r="E107">
+        <v>8154</v>
       </c>
       <c r="F107">
         <v>2</v>
@@ -7813,20 +7799,20 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="28" t="s">
+      <c r="A108" t="s">
         <v>191</v>
       </c>
       <c r="B108">
         <v>35</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="147">
         <v>7</v>
       </c>
       <c r="D108" s="146">
         <v>45859</v>
       </c>
-      <c r="E108" s="33">
-        <v>9056.7604868871877</v>
+      <c r="E108">
+        <v>8368</v>
       </c>
       <c r="F108">
         <v>2</v>
@@ -7836,20 +7822,20 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="28" t="s">
+      <c r="A109" t="s">
         <v>189</v>
       </c>
       <c r="B109">
         <v>36</v>
       </c>
-      <c r="C109">
+      <c r="C109" s="147">
         <v>7</v>
       </c>
       <c r="D109" s="146">
         <v>45859</v>
       </c>
-      <c r="E109" s="33">
-        <v>9679.0183120639485</v>
+      <c r="E109">
+        <v>8944</v>
       </c>
       <c r="F109">
         <v>2</v>
@@ -7858,10 +7844,33 @@
         <v>1</v>
       </c>
     </row>
+    <row r="110" spans="1:7" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="147" t="s">
+        <v>236</v>
+      </c>
+      <c r="B110" s="147">
+        <v>36</v>
+      </c>
+      <c r="C110" s="147">
+        <v>7</v>
+      </c>
+      <c r="D110" s="148">
+        <v>45859</v>
+      </c>
+      <c r="E110" s="147">
+        <v>7992</v>
+      </c>
+      <c r="F110" s="147">
+        <v>2</v>
+      </c>
+      <c r="G110" s="147">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A38:G109">
-    <sortCondition ref="B38:B109"/>
-    <sortCondition ref="G38:G109"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A39:G110">
+    <sortCondition ref="B39:B110"/>
+    <sortCondition ref="G39:G110"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>